<commit_message>
update memmo and mac
</commit_message>
<xml_diff>
--- a/memo/memo.xlsx
+++ b/memo/memo.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25721"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrjam\OneDrive\เดสก์ท็อป\Jame\code\tools_code_memo\memo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB8B64E1-DAB7-4713-8F0D-E7C10133AADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E91DCED-026A-43B4-A8B5-2FA73E343B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vue" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="port" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
+    <sheet name="port" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>command</t>
   </si>
@@ -47,7 +49,7 @@
   </si>
   <si>
     <t>&lt;v-row  justify="center"&gt;
-    &lt;v-col cols='12' lg='6' xl='5'&gt;lllll&lt;/v-col&gt;
+    &lt;v-col cols='12' md='6' xl='5'&gt;lllll&lt;/v-col&gt;
 &lt;/v-row&gt;</t>
   </si>
   <si>
@@ -130,20 +132,6 @@
         &lt;/v-row&gt;</t>
   </si>
   <si>
-    <t>$f</t>
-  </si>
-  <si>
-    <t>exports.fetchLive = (req, res, next) =&gt; {
-  auth.getUserId(req.headers.authorization, (id, _) =&gt; {
-    let sql = ``;
-    db.query(sql, (err, results) =&gt; {
-      if (err) return next(err);
-      res.json(resp(true, results.rows, null, null));
-    });
-  });
-};</t>
-  </si>
-  <si>
     <t>@c</t>
   </si>
   <si>
@@ -165,7 +153,7 @@
                     &lt;/div&gt;</t>
   </si>
   <si>
-    <t>#f</t>
+    <t>#f_f</t>
   </si>
   <si>
     <t>fetchData() {
@@ -186,7 +174,7 @@
     },</t>
   </si>
   <si>
-    <t>#p</t>
+    <t>#f_po</t>
   </si>
   <si>
     <t>postData() {
@@ -271,6 +259,243 @@
     },</t>
   </si>
   <si>
+    <t>#v-pag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   v-if="index &lt; itemPP * page &amp;&amp; itemPP * (page - 1) - 1 &lt; index"
+    &lt;div class="text-center py-10"&gt;
+      &lt;v-pagination
+        v-model="page"
+        :length="news == null ? 0 : Math.ceil(news.length / itemPP)"
+      &gt;&lt;/v-pagination&gt;&lt;/div&gt;
+      itemPP: 12,
+      page: 1,
+      news: null,</t>
+  </si>
+  <si>
+    <t>!async</t>
+  </si>
+  <si>
+    <t>exports.fetchHistory = (req, res, next) =&gt; {
+    auth.getUserId(req.headers.authorization, (id, _) =&gt; {
+        req.getConnection((err, connection) =&gt; {
+            if (err) return next(err);
+            async function productQuery() {
+                let sql = `select * from dp_product where id =${req.params.id} AND owner_id=${id};`;
+                return new Promise(resolve =&gt; {
+                    connection.query(sql, (err, results) =&gt; {
+                        if (err) return next(err);
+                        resolve(results[0]);
+                    });
+                });
+            }
+            async function historyQuery() {
+                let sql = `select * from dp_product_history 
+                where product_id =${req.params.id}
+                ORDER BY date DESC;`;
+                return new Promise(resolve =&gt; {
+                    connection.query(sql, (err, results) =&gt; {
+                        if (err) return next(err);
+                        resolve(results);
+                    });
+                });
+            }
+            async function main() {
+                let product = await productQuery();
+                let history = await historyQuery();
+                let results = {
+                    product: product,
+                    history: history,
+                };
+                res.json(resp(true, results, null, null));
+            }
+            main();
+        })
+    })
+};</t>
+  </si>
+  <si>
+    <t>!b_f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+exports.fetch = (req, res, next) =&gt; {
+    auth.getUserId(req.headers.authorization, (id, _) =&gt; {
+        let sql = `select * from dp_product
+            left join (select id brand_id,name brand_name from dp_car_brand)brand on brand.brand_id = dp_product.brand_id
+            left join (select id model_id,name model_name from dp_car_model)model on model.model_id = dp_product.model_id
+            left join (select id year_id,name year_name from dp_car_year)year on year.year_id = dp_product.year_id
+            WHERE owner_id = ${id};`;
+        req.getConnection((err, connection) =&gt; {
+            if (err) return next(err);
+            connection.query(sql, (err, results) =&gt; {
+                if (err) return next(err);
+                res.json(resp(true, results, null, null));
+            });
+        });
+    });
+};
+</t>
+  </si>
+  <si>
+    <t>!b_po</t>
+  </si>
+  <si>
+    <t>exports.create = (req, res, next) =&gt; {
+    auth.getUserId(req.headers.authorization, (id, _) =&gt; {
+        let {
+            body
+        } = req;
+        body.owner_id = id
+        console.log(body);
+        let sql = `INSERT INTO dp_product SET ?;`;
+        body.image_list = JSON.stringify(body.image_list);
+        body.keyword = JSON.stringify(body.keyword);
+        req.getConnection((err, connection) =&gt; {
+            if (err) return next(err);
+            connection.query(sql, body, (err, _) =&gt; {
+                if (err) return next(err);
+                res.json(resp(true, null, null, null));
+            });
+        });
+    });
+};</t>
+  </si>
+  <si>
+    <t>!b_pu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+exports.edit = (req, res, next) =&gt; {
+    let {
+        body
+    } = req;
+    auth.getUserId(req.headers.authorization, (id, _) =&gt; {
+        let sql = `UPDATE du_shop SET ? WHERE owner_id=${id};`;
+        body.image_list = JSON.stringify(body.image_list)
+        req.getConnection((err, connection) =&gt; {
+            if (err) return next(err);
+            connection.query(sql, body, (err, _) =&gt; {
+                if (err) return next(err);
+                res.json(resp(true, null, null, null));
+            });
+        });
+    })
+};</t>
+  </si>
+  <si>
+    <t>!ms_c</t>
+  </si>
+  <si>
+    <t>CREATE TABLE dp_product (
+    id int NOT NULL AUTO_INCREMENT,
+    name CHAR(30) NOT NULL,
+    delivery_charge int NOT NULL,
+    image_url TEXT,
+    image_list JSON NOT NULL DEFAULT (JSON_ARRAY()),
+    year_id int,
+    PRIMARY KEY (id),
+    FOREIGN KEY (year_id) REFERENCES dp_car_year(id)
+);</t>
+  </si>
+  <si>
+    <t>!ms_i</t>
+  </si>
+  <si>
+    <t>INSERT INTO dp_product (name)
+VALUES ('test Product');</t>
+  </si>
+  <si>
+    <t>du_shop</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>int gen</t>
+  </si>
+  <si>
+    <t>owner_id</t>
+  </si>
+  <si>
+    <t>rela</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>image_url</t>
+  </si>
+  <si>
+    <t>image_list</t>
+  </si>
+  <si>
+    <t>details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use paco;
+-- DROP TABLE dp_product;
+-- CREATE TABLE dp_product (
+--     id int NOT NULL AUTO_INCREMENT,
+--     name CHAR(30) NOT NULL,
+--     price double NOT NULL,
+--     delivery_charge double NOT NULL,
+--     weight double NOT NULL,
+--     discount double,
+--     
+--     image_url TEXT,
+--     sub_product_detail TEXT ,
+--     product_detail TEXT,
+--     
+--     keyword JSON NOT NULL DEFAULT (JSON_ARRAY()),
+--     image_list JSON NOT NULL DEFAULT (JSON_ARRAY()),
+--     
+--     insurance TEXT,
+--     period_insurance TEXT,
+--     
+--     brand_id int,
+--     engine_id int,
+--     model_id int,
+--     submodel_id int,
+--     year_id int,
+--     
+--     main_id int,
+--     sub_id int,
+--     type_id int,
+--     owner_id int NOT NULL,
+--     PRIMARY KEY (id),
+--     FOREIGN KEY (owner_id) REFERENCES du_user(id),
+--     FOREIGN KEY (brand_id) REFERENCES dp_car_brand(id),
+--     FOREIGN KEY (engine_id) REFERENCES dp_car_engine(id),
+--     FOREIGN KEY (model_id) REFERENCES dp_car_model(id),
+--     FOREIGN KEY (submodel_id) REFERENCES dp_car_submodel(id),
+--     FOREIGN KEY (year_id) REFERENCES dp_car_year(id),
+--     FOREIGN KEY (main_id) REFERENCES dp_category_main(id),
+--     FOREIGN KEY (sub_id) REFERENCES dp_category_sub(id),
+-- 	FOREIGN KEY (type_id) REFERENCES dp_category_type(id)
+-- );
+-- INSERT INTO dp_product (name, price,delivery_charge,weight,discount, brand_id, engine_id,model_id,submodel_id,year_id,main_id,sub_id,type_id)
+-- VALUES ('test Product',1150,10,10,0,1,1,1,1,1, NULL ,1, 1 );
+-- INSERT INTO dp_product(name, price, delivery_charge, weight, discount, insurance_id, brand_id, engine_id, model_id, submodel_id, year_id, main_id, type_id, sub_id, image_url, image_list, product_detail, sub_product_detail, keyword) VALUES ('asdasd', 0, 0, 0, 0, 1, 1, null, null, null, null, 2, null, null, 'paco/product/1664285058050_mock.png', paco/product/1664285068059_favicon.ico,paco/product/1664285075324_mock1.png, 'sdasdasd', 'asdasda', )
+-- select * from dp_product
+-- left join (select id,name brand_name from dp_car_brand)brand on brand.id = dp_product.brand_id
+-- left join (select id,name model_name from dp_car_model)model on model.id = dp_product.model_id
+-- left join (select id,name year_name from dp_car_year)year on year.id = dp_product.year_id
+-- left join (select id,name submodel_name from dp_car_submodel)submodel on submodel.id = dp_product.submodel_id
+-- left join (select id,name engine_name from dp_car_engine)engine on engine.id = dp_product.engine_id
+-- left join (select id,name main_name from dp_category_main)main on main.id = dp_product.main_id
+-- left join (select id,name type_name from dp_category_type)type on type.id = dp_product.type_id
+-- left join (select id,name sub_name from dp_category_sub)sub on year.id = dp_product.sub_id
+-- amount
+-- ALTER TABLE dp_product
+-- ADD COLUMN amount double NOT NULL default 0 AFTER name;
+-- select * from dp_product;
+</t>
+  </si>
+  <si>
     <t xml:space="preserve"> &lt;v-tabs-items id="custom-tab-items" v-model="tab"&gt;</t>
   </si>
   <si>
@@ -354,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -372,6 +597,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,10 +906,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -754,52 +982,100 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="150">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="10" spans="1:2" ht="18" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="198">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="255">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="339">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="409.6">
       <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="167.25">
+      <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="409.6">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="381.75">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="336">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="321">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="167.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30.75">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -809,6 +1085,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA5A934-41E9-4583-960E-66CC704D77CA}">
+  <dimension ref="A2:D8"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="A2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C5A473-DD18-4003-B607-2D447F252876}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="409.6">
+      <c r="A1" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E16338-CFE0-4ED2-BB54-C8A106BB9F2C}">
   <dimension ref="D9:D11"/>
   <sheetViews>
@@ -820,17 +1181,17 @@
   <sheetData>
     <row r="9" spans="4:4">
       <c r="D9" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="4:4">
       <c r="D10" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="4:4" ht="210">
       <c r="D11" s="3" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -838,7 +1199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B51138-BDDF-48DE-A522-B3F2D4FDDC8B}">
   <dimension ref="A2:C9"/>
   <sheetViews>
@@ -850,7 +1211,7 @@
   <sheetData>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B2">
         <v>2004</v>
@@ -861,7 +1222,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B3">
         <v>2005</v>
@@ -869,7 +1230,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>2006</v>
@@ -880,7 +1241,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>2007</v>
@@ -888,7 +1249,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B6">
         <v>2008</v>
@@ -899,7 +1260,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B7">
         <v>2009</v>
@@ -910,7 +1271,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B8">
         <v>2012</v>
@@ -918,7 +1279,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="B9">
         <v>2014</v>

</xml_diff>